<commit_message>
Fully functional Box Plot
</commit_message>
<xml_diff>
--- a/labs/Lab12/Source_Data.xlsx
+++ b/labs/Lab12/Source_Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\young\Documents\GitHub\advstatistics-labs\labs\lab11\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\young\Documents\GitHub\advstatistics-labs\labs\Lab12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEBB5EBC-73F1-4C1F-82AA-8E25501AB168}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2391B88-947E-426B-A72A-368D74F826F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1184,10 +1184,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:J82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1227,7 +1228,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -1259,7 +1260,7 @@
         <v>3.3219758819999998</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -1291,7 +1292,7 @@
         <v>1.8926102010000001</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -1323,7 +1324,7 @@
         <v>1.620176101</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -1355,7 +1356,7 @@
         <v>2.9051305620000001</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -1387,7 +1388,7 @@
         <v>2.775163177</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
@@ -1419,7 +1420,7 @@
         <v>2.2854984800000002</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -1451,7 +1452,7 @@
         <v>1.9504596750000001</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -1483,7 +1484,7 @@
         <v>3.2059308930000001</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
@@ -1611,7 +1612,7 @@
         <v>1.718626228</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>29</v>
       </c>
@@ -1931,7 +1932,7 @@
         <v>1.1517397760000001</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>41</v>
       </c>
@@ -1995,7 +1996,7 @@
         <v>2.2666881860000001</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>44</v>
       </c>
@@ -2027,7 +2028,7 @@
         <v>4.2729934749999998</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>45</v>
       </c>
@@ -2059,7 +2060,7 @@
         <v>4.7558233369999998</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>46</v>
       </c>
@@ -2091,7 +2092,7 @@
         <v>2.916795187</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>47</v>
       </c>
@@ -2123,7 +2124,7 @@
         <v>3.1228219429999999</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>49</v>
       </c>
@@ -2155,7 +2156,7 @@
         <v>4.553028962</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>51</v>
       </c>
@@ -2187,7 +2188,7 @@
         <v>5.5295621129999999</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>52</v>
       </c>
@@ -2219,7 +2220,7 @@
         <v>2.5962381680000002</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>53</v>
       </c>
@@ -2251,7 +2252,7 @@
         <v>1.427450023</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>55</v>
       </c>
@@ -2283,7 +2284,7 @@
         <v>4.8806316609999998</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>56</v>
       </c>
@@ -2315,7 +2316,7 @@
         <v>1.8978548740000001</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>57</v>
       </c>
@@ -2347,7 +2348,7 @@
         <v>5.3720879679999998</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>58</v>
       </c>
@@ -2379,7 +2380,7 @@
         <v>3.562723284</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>59</v>
       </c>
@@ -2411,7 +2412,7 @@
         <v>4.891408814</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>60</v>
       </c>
@@ -2443,7 +2444,7 @@
         <v>5.3637776180000003</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>61</v>
       </c>
@@ -2475,7 +2476,7 @@
         <v>3.4281519889999998</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>62</v>
       </c>
@@ -2507,7 +2508,7 @@
         <v>4.6076338459999997</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>63</v>
       </c>
@@ -2539,7 +2540,7 @@
         <v>3.082974213</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>64</v>
       </c>
@@ -2699,7 +2700,7 @@
         <v>2.197162069</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>71</v>
       </c>
@@ -2795,7 +2796,7 @@
         <v>2.462249146</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>74</v>
       </c>
@@ -2827,7 +2828,7 @@
         <v>3.4793082970000002</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>75</v>
       </c>
@@ -3179,7 +3180,7 @@
         <v>2.5694022730000001</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>86</v>
       </c>
@@ -3371,7 +3372,7 @@
         <v>1.36416903</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>92</v>
       </c>
@@ -3435,7 +3436,7 @@
         <v>1.5652581459999999</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>94</v>
       </c>
@@ -3499,7 +3500,7 @@
         <v>2.829956202</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>96</v>
       </c>
@@ -3531,7 +3532,7 @@
         <v>4.02404428</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>97</v>
       </c>
@@ -3627,7 +3628,7 @@
         <v>3.0178694410000002</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>100</v>
       </c>
@@ -3659,7 +3660,7 @@
         <v>5.3901605119999996</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>101</v>
       </c>
@@ -3691,7 +3692,7 @@
         <v>4.9789418689999998</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>102</v>
       </c>
@@ -3723,7 +3724,7 @@
         <v>5.0559677130000003</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>103</v>
       </c>
@@ -3755,7 +3756,7 @@
         <v>4.4167113550000003</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>104</v>
       </c>
@@ -3820,7 +3821,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J82" xr:uid="{6F63531B-75A6-4DA4-B153-57884F784F53}"/>
+  <autoFilter ref="A1:J82" xr:uid="{6F63531B-75A6-4DA4-B153-57884F784F53}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="POST"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>